<commit_message>
2661.firstCompleteIndex & 2662.minimumCost & lcp.79.extractMantra
</commit_message>
<xml_diff>
--- a/Leetcode.xlsx
+++ b/Leetcode.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2softcode\shoran\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BC3B7F-5BD8-4DBB-ADB6-58D82E580F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C516DEAD-F9F4-4564-B5B2-54789AC5D8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2106. 摘水果" sheetId="1" r:id="rId1"/>
+    <sheet name="2662. 前往目标的最小代价" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>[[0,7],[7,4],[9,10],[12,6],[14,8],[16,5],[17,8],[19,4],[20,1],[21,3],[24,3],[25,3],[26,1],[28,10],[30,9],[31,6],[32,1],[37,5],[40,9]]
 21
@@ -36,12 +37,44 @@
     <t>[[5,8],[7,7],[8,7],[15,5],[18,8],[19,3],[25,4],[26,1],[34,10],[38,3],[39,4],[40,5]], 6, 19   34 VS 38</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>[1,1] [10,4] [[4,2,1,1,3],[1,2,7,4,4],[10,3,6,1,2],[6,1,1,2,3]]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +87,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -77,14 +117,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -367,29 +409,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -547,22 +589,22 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -668,4 +710,204 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039CA449-435A-41C7-A79C-2A58FF75AF25}">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1.2</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4.2</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6.1</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>